<commit_message>
Automatische test-sync: 2025-08-14 19:05:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -735,8 +735,60 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>planning@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-08-14 19:05:16</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -756,7 +808,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -764,17 +816,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -816,7 +868,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:24:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -787,8 +787,60 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:24:08</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -808,7 +860,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -816,17 +868,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -868,7 +920,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -839,8 +839,60 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:26:24</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -860,7 +912,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -868,17 +920,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -920,7 +972,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:27:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -891,8 +891,60 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:27:00</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -912,7 +964,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -920,17 +972,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -972,7 +1024,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:28:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -943,8 +943,60 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:28:36</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -964,7 +1016,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -972,17 +1024,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1024,7 +1076,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -995,8 +995,60 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Nieuwe bestelling</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>planning@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Wil je 200 stuks M8-bouten bestellen bij onze leverancier?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:30:43</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1016,7 +1068,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1024,17 +1076,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1076,7 +1128,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1047,8 +1047,60 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:32:52</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1068,7 +1120,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1076,17 +1128,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1128,7 +1180,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:37:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1099,8 +1099,60 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:37:26</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1120,7 +1172,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1128,17 +1180,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1153,7 +1205,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1183,6 +1235,16 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:39:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1151,8 +1151,60 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Nieuwe bestelling</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>planning@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Wil je 200 stuks M8-bouten bestellen bij onze leverancier?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:39:34</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1172,7 +1224,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1180,17 +1232,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J10">
+  <conditionalFormatting sqref="J2:J11">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1205,7 +1257,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1245,6 +1297,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:41:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1203,8 +1203,60 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:41:44</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1224,7 +1276,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1232,17 +1284,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1257,7 +1309,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1307,6 +1359,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1255,8 +1255,120 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Undelivered Mail Returned to Sender</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailer-daemon@mail.zoho.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>This message was created automatically by mail delivery software.
+ A message that you sent could not be delivered to one or more of its recipients. This is a permanent error. 
+support@testbedrijf123.nl, ERROR CODE :550 - 5.0.0 Invalid Recipients.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Geachte afzender,
+Hartelijk dank voor uw bericht. 
+Het lijkt erop dat uw e-mail niet correct is afgeleverd bij onze support@testbedrijf123.nl mailbox vanwege een fout met betrekking tot ongeldige ontvangers (ERROR CODE: 550 - 5.0.0). 
+Om dit probleem te verhelpen, verzoeken wij u vriendelijk om de e-mail opnieuw te verzenden en ervoor te zorgen dat het e-mailadres support@testbedrijf123.nl correct is ingevoerd in de ontvangerlijst. Mocht u verdere hulp nodig hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent bij Testbedrijf123</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:43:57</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>CE-certificaten verzoek</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>inkoop@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Kun je mij de CE-certificaten van de EcoPro-700 sturen?</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Kwaliteit / Certificaten</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar kwaliteit@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:44:07</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1276,7 +1388,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1284,17 +1396,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H14">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I14">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J12">
+  <conditionalFormatting sqref="J2:J14">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1309,7 +1421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1342,17 +1454,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1362,10 +1474,20 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kwaliteit / Certificaten</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:52:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1367,8 +1367,60 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:52:47</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1388,7 +1440,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1396,17 +1448,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H15">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I15">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14">
+  <conditionalFormatting sqref="J2:J15">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1448,7 +1500,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:55:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1419,8 +1419,60 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Nieuwe bestelling</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>planning@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Wil je 200 stuks M8-bouten bestellen bij onze leverancier?</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:54:57</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1440,7 +1492,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1448,17 +1500,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H15">
+  <conditionalFormatting sqref="H2:H16">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I15">
+  <conditionalFormatting sqref="I2:I16">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J15">
+  <conditionalFormatting sqref="J2:J16">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1500,7 +1552,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:57:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1471,8 +1471,60 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:57:06</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1492,7 +1544,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1500,17 +1552,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J16">
+  <conditionalFormatting sqref="J2:J17">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1552,7 +1604,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 20:59:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1523,8 +1523,60 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CE-certificaten verzoek</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>inkoop@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Kun je mij de CE-certificaten van de EcoPro-700 sturen?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar kwaliteit@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-08-14 20:59:16</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1544,7 +1596,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1552,17 +1604,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1604,7 +1656,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:01:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1575,8 +1575,60 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Terugbetaling</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>support@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Ik heb mijn retour gestuurd maar nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar retour@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:01:26</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1596,7 +1648,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1604,17 +1656,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H18">
+  <conditionalFormatting sqref="H2:H19">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I18">
+  <conditionalFormatting sqref="I2:I19">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J18">
+  <conditionalFormatting sqref="J2:J19">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1656,7 +1708,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:03:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1627,8 +1627,60 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klachten@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:03:37</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1648,7 +1700,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1656,17 +1708,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H19">
+  <conditionalFormatting sqref="H2:H20">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I19">
+  <conditionalFormatting sqref="I2:I20">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J19">
+  <conditionalFormatting sqref="J2:J20">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1708,7 +1760,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:13:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1679,8 +1679,60 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:13:48</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1700,7 +1752,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1708,17 +1760,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
+  <conditionalFormatting sqref="I2:I21">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J20">
+  <conditionalFormatting sqref="J2:J21">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1760,7 +1812,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:16:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1731,8 +1731,60 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Nieuwe bestelling</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>planning@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Wil je 200 stuks M8-bouten bestellen bij onze leverancier?</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:15:54</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1752,7 +1804,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1760,17 +1812,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="H2:H22">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I22">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J21">
+  <conditionalFormatting sqref="J2:J22">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1812,7 +1864,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:18:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1783,8 +1783,60 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:18:05</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1804,7 +1856,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1812,17 +1864,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H22">
+  <conditionalFormatting sqref="H2:H23">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I22">
+  <conditionalFormatting sqref="I2:I23">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J22">
+  <conditionalFormatting sqref="J2:J23">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1864,7 +1916,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:20:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1835,8 +1835,60 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CE-certificaten verzoek</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>inkoop@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Kun je mij de CE-certificaten van de EcoPro-700 sturen?</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar kwaliteit@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:20:14</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D23">
+  <conditionalFormatting sqref="D2:D24">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1856,7 +1908,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="G2:G24">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1864,17 +1916,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H23">
+  <conditionalFormatting sqref="H2:H24">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I23">
+  <conditionalFormatting sqref="I2:I24">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J23">
+  <conditionalFormatting sqref="J2:J24">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1916,7 +1968,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:22:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1887,8 +1887,60 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>INTERN – Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:22:16</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D24">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1908,7 +1960,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G24">
+  <conditionalFormatting sqref="G2:G25">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1916,17 +1968,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H24">
+  <conditionalFormatting sqref="H2:H25">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I24">
+  <conditionalFormatting sqref="I2:I25">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J24">
+  <conditionalFormatting sqref="J2:J25">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1941,7 +1993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2011,6 +2063,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>INTERN – Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1939,8 +1939,60 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>INTERN – Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:25:51</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1960,7 +2012,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1968,17 +2020,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H25">
+  <conditionalFormatting sqref="H2:H26">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I25">
+  <conditionalFormatting sqref="I2:I26">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J25">
+  <conditionalFormatting sqref="J2:J26">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1993,7 +2045,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2073,6 +2125,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>INTERN – Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1991,8 +1991,60 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:33:21</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2012,7 +2064,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2020,17 +2072,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H26">
+  <conditionalFormatting sqref="H2:H27">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I26">
+  <conditionalFormatting sqref="I2:I27">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J26">
+  <conditionalFormatting sqref="J2:J27">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2072,7 +2124,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:36:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2043,8 +2043,60 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:36:25</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2064,7 +2116,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G28">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2072,17 +2124,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H27">
+  <conditionalFormatting sqref="H2:H28">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I27">
+  <conditionalFormatting sqref="I2:I28">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J27">
+  <conditionalFormatting sqref="J2:J28">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2124,7 +2176,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:40:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2095,8 +2095,60 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:39:57</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D28">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2116,7 +2168,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G28">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2124,17 +2176,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H28">
+  <conditionalFormatting sqref="H2:H29">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I28">
+  <conditionalFormatting sqref="I2:I29">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J28">
+  <conditionalFormatting sqref="J2:J29">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2176,7 +2228,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:42:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2147,8 +2147,60 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:42:13</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2168,7 +2220,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2176,17 +2228,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H29">
+  <conditionalFormatting sqref="H2:H30">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I29">
+  <conditionalFormatting sqref="I2:I30">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J29">
+  <conditionalFormatting sqref="J2:J30">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2228,7 +2280,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:49:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2199,8 +2199,60 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:49:21</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D31">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2220,7 +2272,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2228,17 +2280,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H30">
+  <conditionalFormatting sqref="H2:H31">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I30">
+  <conditionalFormatting sqref="I2:I31">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J30">
+  <conditionalFormatting sqref="J2:J31">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2280,7 +2332,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:54:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2251,8 +2251,60 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:54:22</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D31">
+  <conditionalFormatting sqref="D2:D32">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2272,7 +2324,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G31">
+  <conditionalFormatting sqref="G2:G32">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2280,17 +2332,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H31">
+  <conditionalFormatting sqref="H2:H32">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I31">
+  <conditionalFormatting sqref="I2:I32">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J31">
+  <conditionalFormatting sqref="J2:J32">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2332,7 +2384,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:55:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2303,8 +2303,60 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:55:45</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D32">
+  <conditionalFormatting sqref="D2:D33">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2324,7 +2376,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G32">
+  <conditionalFormatting sqref="G2:G33">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2332,17 +2384,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H32">
+  <conditionalFormatting sqref="H2:H33">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I32">
+  <conditionalFormatting sqref="I2:I33">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J32">
+  <conditionalFormatting sqref="J2:J33">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2384,7 +2436,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 21:58:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2355,8 +2355,60 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Nieuwe bestelling</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>planning@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Wil je 200 stuks M8-bouten bestellen bij onze leverancier?</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-08-14 21:57:54</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D33">
+  <conditionalFormatting sqref="D2:D34">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2376,7 +2428,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G33">
+  <conditionalFormatting sqref="G2:G34">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2384,17 +2436,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H33">
+  <conditionalFormatting sqref="H2:H34">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I33">
+  <conditionalFormatting sqref="I2:I34">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J33">
+  <conditionalFormatting sqref="J2:J34">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2436,7 +2488,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 22:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2407,8 +2407,60 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-08-14 22:00:01</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D34">
+  <conditionalFormatting sqref="D2:D35">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2428,7 +2480,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G34">
+  <conditionalFormatting sqref="G2:G35">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2436,17 +2488,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H34">
+  <conditionalFormatting sqref="H2:H35">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I34">
+  <conditionalFormatting sqref="I2:I35">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J34">
+  <conditionalFormatting sqref="J2:J35">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2488,7 +2540,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 22:02:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2459,8 +2459,60 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>CE-certificaten verzoek</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>inkoop@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Kun je mij de CE-certificaten van de EcoPro-700 sturen?</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar kwaliteit@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2025-08-14 22:02:10</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D35">
+  <conditionalFormatting sqref="D2:D36">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2480,7 +2532,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G35">
+  <conditionalFormatting sqref="G2:G36">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2488,17 +2540,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H35">
+  <conditionalFormatting sqref="H2:H36">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I35">
+  <conditionalFormatting sqref="I2:I36">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J35">
+  <conditionalFormatting sqref="J2:J36">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2540,7 +2592,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 22:04:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2511,8 +2511,60 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Terugbetaling</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>support@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Ik heb mijn retour gestuurd maar nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar retour@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2025-08-14 22:04:19</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D36">
+  <conditionalFormatting sqref="D2:D37">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2532,7 +2584,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G36">
+  <conditionalFormatting sqref="G2:G37">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2540,17 +2592,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H36">
+  <conditionalFormatting sqref="H2:H37">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I36">
+  <conditionalFormatting sqref="I2:I37">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J36">
+  <conditionalFormatting sqref="J2:J37">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2592,7 +2644,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 22:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2563,8 +2563,60 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klachten@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2025-08-14 22:06:29</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D37">
+  <conditionalFormatting sqref="D2:D38">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2584,7 +2636,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G37">
+  <conditionalFormatting sqref="G2:G38">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2592,17 +2644,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H37">
+  <conditionalFormatting sqref="H2:H38">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I37">
+  <conditionalFormatting sqref="I2:I38">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J37">
+  <conditionalFormatting sqref="J2:J38">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2644,7 +2696,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 22:08:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2615,8 +2615,60 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Datasheet opvragen</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>retour@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar documentatie@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2025-08-14 22:08:40</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D38">
+  <conditionalFormatting sqref="D2:D39">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2636,7 +2688,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G38">
+  <conditionalFormatting sqref="G2:G39">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2644,17 +2696,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H38">
+  <conditionalFormatting sqref="H2:H39">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I38">
+  <conditionalFormatting sqref="I2:I39">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J38">
+  <conditionalFormatting sqref="J2:J39">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2696,7 +2748,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 22:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2667,8 +2667,60 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Vraag over product</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>documentatie@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Is de EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2025-08-14 22:10:52</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D39">
+  <conditionalFormatting sqref="D2:D40">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2688,7 +2740,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G39">
+  <conditionalFormatting sqref="G2:G40">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2696,17 +2748,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H39">
+  <conditionalFormatting sqref="H2:H40">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I39">
+  <conditionalFormatting sqref="I2:I40">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J39">
+  <conditionalFormatting sqref="J2:J40">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2748,7 +2800,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 22:13:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2719,8 +2719,60 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Opvolging retour</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Hebben jullie al nieuws over mijn retour?</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klantenservice@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2025-08-14 22:13:04</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D40">
+  <conditionalFormatting sqref="D2:D41">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2740,7 +2792,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G40">
+  <conditionalFormatting sqref="G2:G41">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2748,17 +2800,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H40">
+  <conditionalFormatting sqref="H2:H41">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I40">
+  <conditionalFormatting sqref="I2:I41">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J40">
+  <conditionalFormatting sqref="J2:J41">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2800,7 +2852,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-14 22:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-14.xlsx
+++ b/logs/mail_log_2025-08-14.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2771,8 +2771,60 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Algemene vraag</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>klachten@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Kunnen jullie mij meer informatie sturen over jullie diensten?</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2025-08-14 22:15:18</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D41">
+  <conditionalFormatting sqref="D2:D42">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2792,7 +2844,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G41">
+  <conditionalFormatting sqref="G2:G42">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2800,17 +2852,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H41">
+  <conditionalFormatting sqref="H2:H42">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I41">
+  <conditionalFormatting sqref="I2:I42">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J41">
+  <conditionalFormatting sqref="J2:J42">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2852,7 +2904,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">

</xml_diff>